<commit_message>
Added test support for model year tracking.
</commit_message>
<xml_diff>
--- a/tests/test-aircraft-sales-entries.xlsx
+++ b/tests/test-aircraft-sales-entries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwall\source\repos\plane-finder-app\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b40200003f3f7d9f/Documents/plane-finder-app/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D973642B-2BE0-4E6C-B277-171CC7D11646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{D973642B-2BE0-4E6C-B277-171CC7D11646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FA99EAB-66A2-41C0-B5F1-E63C9F58F217}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{78480001-85EB-4192-A616-A4D77A9E9696}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>id</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>N827DA</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -491,19 +494,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB16BC43-5EB7-4EEF-9DC2-18B6DEECB050}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,28 +517,31 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -545,26 +551,29 @@
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
+        <v>1982</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>150000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I2">
+      <c r="I2" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J2">
         <v>3000</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -574,26 +583,29 @@
       <c r="C3">
         <v>101</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3">
+      <c r="D3">
+        <v>1968</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
         <v>140000</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I3">
+      <c r="I3" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J3">
         <v>2399</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -603,26 +615,29 @@
       <c r="C4">
         <v>102</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4">
+      <c r="D4">
+        <v>1977</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
         <v>230000</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I4">
+      <c r="I4" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J4">
         <v>5000</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1504</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -632,26 +647,29 @@
       <c r="C5">
         <v>103</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
+        <v>1984</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
         <v>200000</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I5">
+      <c r="I5" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J5">
         <v>6000</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1893</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -661,26 +679,29 @@
       <c r="C6">
         <v>104</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
+      <c r="D6">
+        <v>1967</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
         <v>130000</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I6">
+      <c r="I6" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J6">
         <v>8029</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1383</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -690,26 +711,29 @@
       <c r="C7">
         <v>105</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7">
+      <c r="D7">
+        <v>1959</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
         <v>145000</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I7">
+      <c r="I7" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J7">
         <v>7239</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1084</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -719,26 +743,29 @@
       <c r="C8">
         <v>106</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8">
+      <c r="D8">
+        <v>1963</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8">
         <v>160000</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I8">
+      <c r="I8" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J8">
         <v>4828</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>982</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -748,26 +775,29 @@
       <c r="C9">
         <v>107</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9">
+      <c r="D9">
+        <v>1968</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9">
         <v>172343</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I9">
+      <c r="I9" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J9">
         <v>3941</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>729</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -777,26 +807,29 @@
       <c r="C10">
         <v>108</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10">
+      <c r="D10">
+        <v>1970</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10">
         <v>190000</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I10">
+      <c r="I10" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J10">
         <v>3983</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1888</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -806,22 +839,25 @@
       <c r="C11">
         <v>109</v>
       </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11">
+      <c r="D11">
+        <v>1960</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11">
         <v>135000</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="2">
-        <v>44721</v>
-      </c>
-      <c r="I11">
+      <c r="I11" s="2">
+        <v>44721</v>
+      </c>
+      <c r="J11">
         <v>5921</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1683</v>
       </c>
     </row>

</xml_diff>